<commit_message>
Add testimonials to success-stories page and commit profile pictures
- Add Cole H. and Ebuka O. testimonials to success-stories.html
- Add profile pictures for Gavin and Ebuka (testimonials/pictures/)
- Update success stories with clickable cards and scroll padding
- Archive testimonial callout mockups
- Commit testimonial data files (background.txt, google_forms_feedback.xlsx)
</commit_message>
<xml_diff>
--- a/testimonials/google_forms_feedback.xlsx
+++ b/testimonials/google_forms_feedback.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$K$3</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$K$5</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Timestamp</t>
   </si>
@@ -103,6 +103,54 @@
   </si>
   <si>
     <t>Launch: getting the first job or an entry level job</t>
+  </si>
+  <si>
+    <t>chunzeker24@gmail.com</t>
+  </si>
+  <si>
+    <t>The biggest challenge I was facing at the time was lack of upward mobility, and preparedness if the right opportunity came up.</t>
+  </si>
+  <si>
+    <t>I felt stuck and was unsure how to get to the next level of my career. At times it would lead to burnout in my current role because it felt like I would never get another opportunity.</t>
+  </si>
+  <si>
+    <t>The most helpful advice I received was in regards to positioning myself for the next step. I was told to go above and beyond in my current role. That didn’t just mean in the work I do, but also the connections I make. Additionally, I was mentored on proper interviewing skills for when I do get an opportunity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I believe you are very honest and have went through similar experiences as I have. You were specific in your advice and even gave real life suggestions pertaining to my job that would help with career advancement. You know it’s not a one size fits all for advancement and your ability to recognize that and give me the ingredients specific to my aspirations l was very helpful. </t>
+  </si>
+  <si>
+    <t>I received an interview for a promotion. While I didn’t get the job, I got great feedback from the interviewer about my interviewing skills and the only reason I didn’t get the job was there was someone already in line for the position. I have also gotten more recognition on my team as a result of implementing the advice I was given.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It’s hard to put a number on the help received but I think it kickstarted my advancement. I believe I will get a promotion a year or 2 earlier than I would have without the help and advice. I now feel positioned well for the future. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I would say there are many reasons. You are always willing to lend advice, many times based on personal experiences. You also have a history of success and advancement which is always a positive when working with another individual. Most importantly, you are honest and adaptable which helps with framing advice for an individual. </t>
+  </si>
+  <si>
+    <t>chiebukaonyejesi@gmail.com</t>
+  </si>
+  <si>
+    <t>I was starting out as an intern at John Deere and needed to know how to maximize my internship to get a return offer and overall make an impact at the company.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I felt kinda lost and it was something I wanted to overcome at the time. I felt like getting a coach would make it easier to cross that barrier and achieve my plans for the summer faster. </t>
+  </si>
+  <si>
+    <t>You told me not to put myself in a box and just limit my experience/career to John Deere. That's something I was shocked to hear because most people will try to convince you to work for their company but you said there's a lot of opportunities everywhere and I should really try to find what really resonates with me.</t>
+  </si>
+  <si>
+    <t>I felt like you were more raw and didn’t just say generic stuff. You said things and gave feedback that was actually applicable and not just fluff. I like how you also didn’t just jump into giving advice you kind of dug a bit deeper before your responses.</t>
+  </si>
+  <si>
+    <t>I believe I connected with more people at John Deere and also made the most out of my intern summer project because I was in direct contact with my manger. I also started thinking more about my career out of John Deere and continue working fully on the app I was developing because you highlighted everyone's path is different.</t>
+  </si>
+  <si>
+    <t>I would say there has been infact an impact in my career trajectory. I have had some changes in mindset. I think more deeply and broadly about things related to my career now and try not to limit myself or get stuck up on a specific role/company.</t>
+  </si>
+  <si>
+    <t>As I said earlier, he's very raw and wouldn't just tell you things you would like to hear. I believe he would give you realistic and actionable advice and will also adapt it to your current situation.</t>
   </si>
 </sst>
 </file>
@@ -145,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -163,6 +211,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -245,8 +299,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K3" displayName="Form_Responses" name="Form_Responses" id="1">
-  <autoFilter ref="$A$1:$K$3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K5" displayName="Form_Responses" name="Form_Responses" id="1">
+  <autoFilter ref="$A$1:$K$5"/>
   <tableColumns count="11">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -587,6 +641,76 @@
         <v>20</v>
       </c>
     </row>
+    <row r="4" ht="22.5" customHeight="1">
+      <c r="A4" s="8">
+        <v>45984.67118607639</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" ht="22.5" customHeight="1">
+      <c r="A5" s="8">
+        <v>45984.78307002315</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Implement blog functionality with ConvertKit integration
- Create blog index page (blog.html)
- Create 3 blog post templates (blog-post-1, 2, 3)
- Integrate ConvertKit signup forms
- Add custom JS handler for ConvertKit success messages to fix UI feedback loop
</commit_message>
<xml_diff>
--- a/testimonials/google_forms_feedback.xlsx
+++ b/testimonials/google_forms_feedback.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$K$5</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$K$6</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Timestamp</t>
   </si>
@@ -151,6 +151,30 @@
   </si>
   <si>
     <t>As I said earlier, he's very raw and wouldn't just tell you things you would like to hear. I believe he would give you realistic and actionable advice and will also adapt it to your current situation.</t>
+  </si>
+  <si>
+    <t>mucabap@gmail.com</t>
+  </si>
+  <si>
+    <t>Before we started working together, my biggest challenge was feeling stuck in my career development. I had goals and ambitions, but I lacked clarity about the best path forward and the strategies needed to progress with confidence. I also struggled to translate my potential into visible results and didn’t have a structured plan to improve my performance and positioning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I had the ambition to transition from the design field to the software area, but I often felt that I lacked the technical direction, confidence, and clarity to make that change effectively. This created a sense of stagnation, as I knew I had the potential to contribute more strategically to the tech environment but wasn’t fully sure how to bridge the gap between where I was and where I wanted to be. </t>
+  </si>
+  <si>
+    <t>Instead of treating the shift as a leap into the unknown, you helped me break it down into practical steps: identifying the skills I already had that were transferable, mapping the new capabilities I needed to develop, and creating a realistic learning roadmap. This framework gave me clarity, direction, and confidence, and made the transition feel achievable rather than overwhelming</t>
+  </si>
+  <si>
+    <t>Your mentoring style stood out because it wasn’t generic or theoretical — it was personalized, practical, and grounded in real-world experience. Instead of giving broad advice like many others do, you took the time to understand my goals, strengths, and challenges, and then tailored the guidance to my specific situation.</t>
+  </si>
+  <si>
+    <t>I noticed a clear improvement in my productivity and decision-making: started operating with intention, milestones, and measurable progress. This not only accelerated my development but also increased my sense of ownership and confidence in my career evolution.</t>
+  </si>
+  <si>
+    <t>Our work helped me accelerate my transition into the software area, prioritize the right skills, and position myself more strategically in the company. Additionally, your technique on how to use AI the right way has been a game changer for me. Learning how to craft effective prompts and leverage AI thoughtfully has not only improved my technical results but also strengthened my communication, decision-making, and overall professional performance.</t>
+  </si>
+  <si>
+    <t>Mansour is not just about receiving advice — it’s about gaining clarity, structure, and a personalized strategy for real professional growth. He understands your goals deeply, challenges you with the right questions, and provides practical frameworks you can actually apply. His mentoring combines empathy, market experience, and a results-focused mindset. He can provide the guidance that accelerates your development, sharpens how you think, and helps you take confident steps toward your career goals.</t>
   </si>
 </sst>
 </file>
@@ -299,8 +323,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K5" displayName="Form_Responses" name="Form_Responses" id="1">
-  <autoFilter ref="$A$1:$K$5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K6" displayName="Form_Responses" name="Form_Responses" id="1">
+  <autoFilter ref="$A$1:$K$6"/>
   <tableColumns count="11">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -711,6 +735,41 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" ht="22.5" customHeight="1">
+      <c r="A6" s="8">
+        <v>45985.74253560185</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update index video to v2 (mp4, louder volume, smaller size) and add Sarah Korssa photo
</commit_message>
<xml_diff>
--- a/testimonials/google_forms_feedback.xlsx
+++ b/testimonials/google_forms_feedback.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$K$6</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t>Timestamp</t>
   </si>
@@ -175,6 +175,54 @@
   </si>
   <si>
     <t>Mansour is not just about receiving advice — it’s about gaining clarity, structure, and a personalized strategy for real professional growth. He understands your goals deeply, challenges you with the right questions, and provides practical frameworks you can actually apply. His mentoring combines empathy, market experience, and a results-focused mindset. He can provide the guidance that accelerates your development, sharpens how you think, and helps you take confident steps toward your career goals.</t>
+  </si>
+  <si>
+    <t>acverza.jr@gmail.com</t>
+  </si>
+  <si>
+    <t>The main frustration I had was not feeling recognized for the all the work I did on my previous team and not even being sure that doing a good job was gonna take me anywhere in the company so really I was questioning how good of a fit I was to the company at that point. The new job in the US was one last try to find a good place for me within Deere. The main challenge was fitting in with the new team and understanding how to perform my job well while being a good teammate.</t>
+  </si>
+  <si>
+    <t>I felt underappreciated and I was sure things were gonna be similar in the new job. I didn't have any career aspirations at that point, I was just trying to find a team and leadership that would appreciate my effort and work ethic.</t>
+  </si>
+  <si>
+    <t>Your constant positive feedback helped me gain confidence that I was doing a good job and some of our conversations about possible new roles helped me build a better vision of things I could do.</t>
+  </si>
+  <si>
+    <t>I liked how you tried to connect with people and be informal</t>
+  </si>
+  <si>
+    <t>Increased confidence level on my performance that encouraged me to consider new roles above my pay grade.</t>
+  </si>
+  <si>
+    <t>The main impact is that I feel confident my hard work can be recognized at least by some people.</t>
+  </si>
+  <si>
+    <t>If you aspire to play the corporate game to gain influence, Mansour can help you.</t>
+  </si>
+  <si>
+    <t>sarah.korssa@gmail.com</t>
+  </si>
+  <si>
+    <t>I couldn’t put to words what I’ve done</t>
+  </si>
+  <si>
+    <t>Ugh it was a roadblock, an actual pain</t>
+  </si>
+  <si>
+    <t>Yes, I couldn’t have gotten far in my career without your hands on helping with my resume, advice and trusted mentorship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are very knowledgeable and care. You make whoever you mentor more motivated </t>
+  </si>
+  <si>
+    <t>I was getting better offers, easily getting interviews and more</t>
+  </si>
+  <si>
+    <t>$20,000+</t>
+  </si>
+  <si>
+    <t>There isn’t anyone else who’s as knowledgeable and cares that Will can can genuinely help</t>
   </si>
 </sst>
 </file>
@@ -323,8 +371,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K6" displayName="Form_Responses" name="Form_Responses" id="1">
-  <autoFilter ref="$A$1:$K$6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K8" displayName="Form_Responses" name="Form_Responses" id="1">
+  <autoFilter ref="$A$1:$K$8"/>
   <tableColumns count="11">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -770,6 +818,73 @@
         <v>20</v>
       </c>
     </row>
+    <row r="7" ht="22.5" customHeight="1">
+      <c r="A7" s="8">
+        <v>45986.33564960648</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" ht="22.5" customHeight="1">
+      <c r="A8" s="8">
+        <v>45992.82070719908</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add Asjad Pasha client folder with onboarding materials, LinkedIn posts, and testimonial updates
</commit_message>
<xml_diff>
--- a/testimonials/google_forms_feedback.xlsx
+++ b/testimonials/google_forms_feedback.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$K$9</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
   <si>
     <t>Timestamp</t>
   </si>
@@ -223,6 +223,30 @@
   </si>
   <si>
     <t>There isn’t anyone else who’s as knowledgeable and cares that Will can can genuinely help</t>
+  </si>
+  <si>
+    <t>aj.marsiglio@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Before we met and you took over your role as supervisor, my position faced many challenges. The #1 challenge in my mind was the lack of a clear and defined processes for accomplishing my work. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The challenge created chaos not just for my specific role but for my whole team. It was very frustrating coming to work not know if anything had changed since yesterday or if plans were going to change today. It made me reconsider if I wanted to stay in my role. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I believe the most valuable piece of advice that you have given me is to advocate for myself and properly show what I have accomplished. Early on in my career I had my nose down, grinding away at work and projects but once goals were met and accomplished I simply moved on to the next without showing what I had accomplished. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What sets you apart from others is your ability to try to look at things from multiple angles. From what I have seen you genuinely take the time to try to look at an issue or task from many angles and try to get a good representation of how everyone sees it, not just how you see it. I believe that has allowed you to have a better view and provide better, more honest guidance and assistance. </t>
+  </si>
+  <si>
+    <t>I saw an increase in efficiency in my work, an increase of accreditation by showing my work, and an overall higher job satisfaction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working with you definitely helped my career trajectory as it has already impacted me as I am now a grade 7 and doing well. I believe I am setup to continue to move upwards as well. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I would say he does not rush to judgement as he takes his time properly identifying the surface as well as underlying issues of any situation. He creates detailed plans and goals to attack those problems. Most importantly, he gives fair and honest feedback and advice on how to solve a problem or achieve a goal. </t>
   </si>
 </sst>
 </file>
@@ -371,8 +395,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K8" displayName="Form_Responses" name="Form_Responses" id="1">
-  <autoFilter ref="$A$1:$K$8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K9" displayName="Form_Responses" name="Form_Responses" id="1">
+  <autoFilter ref="$A$1:$K$9"/>
   <tableColumns count="11">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -885,6 +909,41 @@
         <v>20</v>
       </c>
     </row>
+    <row r="9" ht="22.5" customHeight="1">
+      <c r="A9" s="8">
+        <v>45994.611641932876</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add social media content, market trends graphics, LinkedIn posts, email templates, discovery call protocol, lead magnet brainstorm, testimonial data, TikTok scripts
</commit_message>
<xml_diff>
--- a/testimonials/google_forms_feedback.xlsx
+++ b/testimonials/google_forms_feedback.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$K$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$K$10</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t>Timestamp</t>
   </si>
@@ -247,6 +247,30 @@
   </si>
   <si>
     <t xml:space="preserve">I would say he does not rush to judgement as he takes his time properly identifying the surface as well as underlying issues of any situation. He creates detailed plans and goals to attack those problems. Most importantly, he gives fair and honest feedback and advice on how to solve a problem or achieve a goal. </t>
+  </si>
+  <si>
+    <t>lukumkulkarni@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giving surface level answers that didn’t show the breadth of my knowledge. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I wasn’t able to convey what was really going on in my projects and important my work was to the project. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The most valuable piece of advice that you gave me was when you told me to try understand the core competency of the STAR question, rather than to loosely fitting my examples to the question. This way I can adapt my situation to specific topics that the interview is assessing, and I can bring out more detail about specifics that interview is inquiring about. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I believe you are a no-nonsense mentor that brings what I need to work on straight to the point without sugarcoating. Sometimes other mentors will guide me in the wrong direction by not saying what I need to work on, because they are trying to not hurt feelings. But you are very direct and can pinpoint exactly what I need to work on, which streamlines the whole session. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I was able to organize my thoughts by first understanding identifying the competency, then working backwards from there.  That even gave me better chances to pick a better story to satisfy the competency. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">My trajectory is upward since you helped me have more deliberate interview answers. I think this is the step in the right direction, but I need to do more work with you to solidify that trajectory. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you want someone to truly guide and asses how well you are doing without giving you sugarcoated feedback, then work with Mansour. He will give you his undivided attention as he deliberately finds ways you can improve your interviewing/career skills. </t>
   </si>
 </sst>
 </file>
@@ -394,9 +418,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K9" displayName="Form_Responses" name="Form_Responses" id="1">
-  <autoFilter ref="$A$1:$K$9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K10" displayName="Form_Responses" name="Form_Responses" id="1">
+  <autoFilter ref="$A$1:$K$10"/>
   <tableColumns count="11">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -944,6 +972,41 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10" ht="22.5" customHeight="1">
+      <c r="A10" s="8">
+        <v>46062.49713708334</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>